<commit_message>
fixed test2, applied requested changes
</commit_message>
<xml_diff>
--- a/tools/variant_analyzer/test-data/mutant_reads_summary_short_trim_test_data_VA.xlsx
+++ b/tools/variant_analyzer/test-data/mutant_reads_summary_short_trim_test_data_VA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="186">
   <si>
     <t>tag</t>
   </si>
@@ -123,7 +123,7 @@
     <t>variant ID</t>
   </si>
   <si>
-    <t>GATAACCTTGCTTCGTGATTAATC</t>
+    <t>GATTGGATAACGTTGTGGCAATTG</t>
   </si>
   <si>
     <t>ab1.ba2</t>
@@ -141,249 +141,249 @@
     <t>A</t>
   </si>
   <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>ACH_TDII_5regions-505-C-A</t>
+  </si>
+  <si>
+    <t>ab2.ba1</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>571</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>ACH_TDII_5regions-571-C-T</t>
+  </si>
+  <si>
+    <t>CCTCCCGGCAGTGCGAAAATGTCA</t>
+  </si>
+  <si>
+    <t>958</t>
+  </si>
+  <si>
     <t>3.1</t>
   </si>
   <si>
-    <t>ACH_TDII_5regions-505-C-A</t>
-  </si>
-  <si>
-    <t>ab2.ba1</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>GATTGGATAACGTTGTGGCAATTG</t>
-  </si>
-  <si>
-    <t>571</t>
-  </si>
-  <si>
-    <t>T</t>
+    <t>ACH_TDII_5regions-958-T-C</t>
+  </si>
+  <si>
+    <t>cvrg (Du Novo)</t>
+  </si>
+  <si>
+    <t>tier 1.1</t>
+  </si>
+  <si>
+    <t>AF 1.1</t>
+  </si>
+  <si>
+    <t>tier 1.2</t>
+  </si>
+  <si>
+    <t>AF 1.2</t>
+  </si>
+  <si>
+    <t>tier 2.1</t>
+  </si>
+  <si>
+    <t>AF 2.1</t>
+  </si>
+  <si>
+    <t>tier 2.2</t>
+  </si>
+  <si>
+    <t>AF 2.2</t>
+  </si>
+  <si>
+    <t>tier 2.3</t>
+  </si>
+  <si>
+    <t>AF 2.3</t>
+  </si>
+  <si>
+    <t>tier 2.4</t>
+  </si>
+  <si>
+    <t>AF 2.4</t>
+  </si>
+  <si>
+    <t>tier 3.1</t>
+  </si>
+  <si>
+    <t>AF 3.1</t>
+  </si>
+  <si>
+    <t>tier 4</t>
+  </si>
+  <si>
+    <t>AF 4</t>
+  </si>
+  <si>
+    <t>AF 1.1-1.2</t>
+  </si>
+  <si>
+    <t>AF 1.1-2.1</t>
+  </si>
+  <si>
+    <t>AF 1.1-2.2</t>
+  </si>
+  <si>
+    <t>AF 1.1-2.3</t>
+  </si>
+  <si>
+    <t>AF 1.1-2.4</t>
+  </si>
+  <si>
+    <t>AF 1.1-3.1</t>
+  </si>
+  <si>
+    <t>AF 1.1-4</t>
+  </si>
+  <si>
+    <t>cvrg (VA)</t>
+  </si>
+  <si>
+    <t>tier count</t>
+  </si>
+  <si>
+    <t>AF (VA)</t>
+  </si>
+  <si>
+    <t>alt. allele (Du Novo)</t>
+  </si>
+  <si>
+    <t>AF (Du Novo)</t>
+  </si>
+  <si>
+    <t>ref. allele (Du Novo)</t>
+  </si>
+  <si>
+    <t>tier</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>Description of tiers with examples</t>
+  </si>
+  <si>
+    <t>Tier 1.1</t>
+  </si>
+  <si>
+    <t>both ab and ba SSCS present (&gt;75% of the sites with alternative base) and minimal FS&gt;=3 for both SSCS in at least one mate</t>
+  </si>
+  <si>
+    <t>AAAAAGATGCCGACTACCTT</t>
+  </si>
+  <si>
+    <t>Chr5:5-20000</t>
+  </si>
+  <si>
+    <t>11068</t>
+  </si>
+  <si>
+    <t>254</t>
+  </si>
+  <si>
+    <t>228</t>
+  </si>
+  <si>
+    <t>287</t>
+  </si>
+  <si>
+    <t>288</t>
+  </si>
+  <si>
+    <t>289</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>4081</t>
+  </si>
+  <si>
+    <t>4098</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Chr5:5-20000-11068-C-G</t>
+  </si>
+  <si>
+    <t>AAAAATGCGTAGAAATATGC</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>268</t>
+  </si>
+  <si>
+    <t>270</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Tier 1.2</t>
+  </si>
+  <si>
+    <t>both ab and ba SSCS present (&gt;75% of the sites with alt. base) and mate pair validation (min. FS=1) and minimal FS&gt;=3 for at least one of the SSCS</t>
+  </si>
+  <si>
+    <t>CTATGACCCGTGAGCCCATG</t>
+  </si>
+  <si>
+    <t>10776</t>
+  </si>
+  <si>
+    <t>132</t>
+  </si>
+  <si>
+    <t>290</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
-    <t>ACH_TDII_5regions-571-C-T</t>
-  </si>
-  <si>
-    <t>CCTCCCGGCAGTGCGAAAATGTCA</t>
-  </si>
-  <si>
-    <t>958</t>
-  </si>
-  <si>
-    <t>ACH_TDII_5regions-958-T-C</t>
-  </si>
-  <si>
-    <t>cvrg (Du Novo)</t>
-  </si>
-  <si>
-    <t>tier 1.1</t>
-  </si>
-  <si>
-    <t>AF 1.1</t>
-  </si>
-  <si>
-    <t>tier 1.2</t>
-  </si>
-  <si>
-    <t>AF 1.2</t>
-  </si>
-  <si>
-    <t>tier 2.1</t>
-  </si>
-  <si>
-    <t>AF 2.1</t>
-  </si>
-  <si>
-    <t>tier 2.2</t>
-  </si>
-  <si>
-    <t>AF 2.2</t>
-  </si>
-  <si>
-    <t>tier 2.3</t>
-  </si>
-  <si>
-    <t>AF 2.3</t>
-  </si>
-  <si>
-    <t>tier 2.4</t>
-  </si>
-  <si>
-    <t>AF 2.4</t>
-  </si>
-  <si>
-    <t>tier 3.1</t>
-  </si>
-  <si>
-    <t>AF 3.1</t>
-  </si>
-  <si>
-    <t>tier 4</t>
-  </si>
-  <si>
-    <t>AF 4</t>
-  </si>
-  <si>
-    <t>AF 1.1-1.2</t>
-  </si>
-  <si>
-    <t>AF 1.1-2.1</t>
-  </si>
-  <si>
-    <t>AF 1.1-2.2</t>
-  </si>
-  <si>
-    <t>AF 1.1-2.3</t>
-  </si>
-  <si>
-    <t>AF 1.1-2.4</t>
-  </si>
-  <si>
-    <t>AF 1.1-3.1</t>
-  </si>
-  <si>
-    <t>AF 1.1-4</t>
-  </si>
-  <si>
-    <t>cvrg (VA)</t>
-  </si>
-  <si>
-    <t>tier count</t>
-  </si>
-  <si>
-    <t>AF (VA)</t>
-  </si>
-  <si>
-    <t>alt. allele (Du Novo)</t>
-  </si>
-  <si>
-    <t>AF (Du Novo)</t>
-  </si>
-  <si>
-    <t>ref. allele (Du Novo)</t>
-  </si>
-  <si>
-    <t>tier</t>
-  </si>
-  <si>
-    <t>count</t>
-  </si>
-  <si>
-    <t>Description of tiers with examples</t>
-  </si>
-  <si>
-    <t>Tier 1.1</t>
-  </si>
-  <si>
-    <t>both ab and ba SSCS present (&gt;75% of the sites with alternative base) and minimal FS&gt;=3 for both SSCS in at least one mate</t>
-  </si>
-  <si>
-    <t>AAAAAGATGCCGACTACCTT</t>
-  </si>
-  <si>
-    <t>Chr5:5-20000</t>
-  </si>
-  <si>
-    <t>11068</t>
-  </si>
-  <si>
-    <t>254</t>
-  </si>
-  <si>
-    <t>228</t>
-  </si>
-  <si>
-    <t>287</t>
-  </si>
-  <si>
-    <t>288</t>
-  </si>
-  <si>
-    <t>289</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>4081</t>
-  </si>
-  <si>
-    <t>4098</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>1.1</t>
-  </si>
-  <si>
-    <t>Chr5:5-20000-11068-C-G</t>
-  </si>
-  <si>
-    <t>AAAAATGCGTAGAAATATGC</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>268</t>
-  </si>
-  <si>
-    <t>270</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>Tier 1.2</t>
-  </si>
-  <si>
-    <t>both ab and ba SSCS present (&gt;75% of the sites with alt. base) and mate pair validation (min. FS=1) and minimal FS&gt;=3 for at least one of the SSCS</t>
-  </si>
-  <si>
-    <t>CTATGACCCGTGAGCCCATG</t>
-  </si>
-  <si>
-    <t>10776</t>
-  </si>
-  <si>
-    <t>132</t>
-  </si>
-  <si>
-    <t>290</t>
-  </si>
-  <si>
     <t>47170</t>
   </si>
   <si>
@@ -426,9 +426,6 @@
     <t>8</t>
   </si>
   <si>
-    <t>2.1</t>
-  </si>
-  <si>
     <t>Tier 2.2</t>
   </si>
   <si>
@@ -436,6 +433,9 @@
   </si>
   <si>
     <t>ATCAGCCATGGCTATTATTG</t>
+  </si>
+  <si>
+    <t>chrom5:5-20000</t>
   </si>
   <si>
     <t>72</t>
@@ -1057,13 +1057,13 @@
         <v>131</v>
       </c>
       <c r="F2">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="G2">
         <v>264</v>
       </c>
       <c r="H2">
-        <v>208</v>
+        <v>263</v>
       </c>
       <c r="I2">
         <v>173</v>
@@ -1078,13 +1078,13 @@
         <v>1</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N2">
         <v>1</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -1096,7 +1096,7 @@
         <v>1</v>
       </c>
       <c r="S2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T2">
         <v>0</v>
@@ -1238,7 +1238,7 @@
     </row>
     <row r="5" spans="1:35">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
         <v>36</v>
@@ -1247,16 +1247,16 @@
         <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="E5">
+        <v>128</v>
       </c>
       <c r="F5">
         <v>217</v>
       </c>
-      <c r="G5" t="s">
-        <v>44</v>
+      <c r="G5">
+        <v>195</v>
       </c>
       <c r="H5">
         <v>284</v>
@@ -1268,19 +1268,19 @@
         <v>39</v>
       </c>
       <c r="K5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -1289,19 +1289,19 @@
         <v>0</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S5">
-        <v>1</v>
-      </c>
-      <c r="T5" t="s">
-        <v>44</v>
+        <v>5</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
       </c>
       <c r="U5">
         <v>0</v>
       </c>
-      <c r="V5" t="s">
-        <v>44</v>
+      <c r="V5">
+        <v>1</v>
       </c>
       <c r="W5">
         <v>1</v>
@@ -1331,15 +1331,15 @@
         <v>1</v>
       </c>
       <c r="AG5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI5" t="s">
         <v>48</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:35">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
         <v>43</v>
@@ -1348,19 +1348,19 @@
         <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="E6">
+        <v>263</v>
+      </c>
+      <c r="F6">
+        <v>263</v>
+      </c>
+      <c r="G6">
+        <v>278.5</v>
+      </c>
+      <c r="H6">
+        <v>283.5</v>
       </c>
       <c r="I6">
         <v>143</v>
@@ -1369,19 +1369,19 @@
         <v>39</v>
       </c>
       <c r="K6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -1390,22 +1390,22 @@
         <v>0</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6" t="s">
-        <v>44</v>
-      </c>
-      <c r="U6" t="s">
-        <v>44</v>
-      </c>
-      <c r="V6" t="s">
-        <v>44</v>
-      </c>
-      <c r="W6" t="s">
-        <v>44</v>
+        <v>2</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
       </c>
       <c r="X6">
         <v>0</v>
@@ -1434,7 +1434,7 @@
     </row>
     <row r="8" spans="1:35">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
         <v>36</v>
@@ -1443,7 +1443,7 @@
         <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8" t="s">
         <v>44</v>
@@ -1461,7 +1461,7 @@
         <v>195</v>
       </c>
       <c r="J8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K8" t="s">
         <v>39</v>
@@ -1527,7 +1527,7 @@
         <v>0</v>
       </c>
       <c r="AG8" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="AI8" t="s">
         <v>52</v>
@@ -1535,7 +1535,7 @@
     </row>
     <row r="9" spans="1:35">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
         <v>43</v>
@@ -1544,7 +1544,7 @@
         <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9">
         <v>96</v>
@@ -1562,7 +1562,7 @@
         <v>195</v>
       </c>
       <c r="J9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K9" t="s">
         <v>39</v>
@@ -1789,10 +1789,10 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1813,31 +1813,31 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
         <v>0.5</v>
       </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
       <c r="U2">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="V2">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X2">
         <v>0.5</v>
@@ -1866,16 +1866,16 @@
     </row>
     <row r="3" spans="1:31">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1914,28 +1914,28 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
         <v>0.5</v>
       </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
       <c r="T3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="U3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="V3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="W3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Y3">
         <v>0.5</v>
@@ -2125,7 +2125,7 @@
         <v>54</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:35">
@@ -2141,7 +2141,7 @@
         <v>58</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:35">
@@ -2173,7 +2173,7 @@
         <v>66</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:35">
@@ -2181,7 +2181,7 @@
         <v>68</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:35">
@@ -2399,10 +2399,10 @@
         <v>104</v>
       </c>
       <c r="AG15" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI15" t="s">
         <v>105</v>
-      </c>
-      <c r="AI15" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:35">
@@ -2502,7 +2502,7 @@
     </row>
     <row r="19" spans="1:35">
       <c r="A19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B19" t="s">
         <v>36</v>
@@ -2535,17 +2535,17 @@
         <v>96</v>
       </c>
       <c r="L19" t="s">
+        <v>107</v>
+      </c>
+      <c r="M19" t="s">
         <v>108</v>
       </c>
-      <c r="M19" t="s">
-        <v>109</v>
-      </c>
       <c r="N19" t="s">
+        <v>107</v>
+      </c>
+      <c r="O19" t="s">
         <v>108</v>
       </c>
-      <c r="O19" t="s">
-        <v>109</v>
-      </c>
       <c r="P19" t="s">
         <v>99</v>
       </c>
@@ -2553,10 +2553,10 @@
         <v>99</v>
       </c>
       <c r="R19" t="s">
+        <v>107</v>
+      </c>
+      <c r="S19" t="s">
         <v>108</v>
-      </c>
-      <c r="S19" t="s">
-        <v>109</v>
       </c>
       <c r="T19" t="s">
         <v>99</v>
@@ -2595,15 +2595,15 @@
         <v>104</v>
       </c>
       <c r="AG19" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI19" t="s">
         <v>105</v>
-      </c>
-      <c r="AI19" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:35">
       <c r="A20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B20" t="s">
         <v>43</v>
@@ -2615,13 +2615,13 @@
         <v>90</v>
       </c>
       <c r="E20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F20" t="s">
+        <v>109</v>
+      </c>
+      <c r="G20" t="s">
         <v>110</v>
-      </c>
-      <c r="F20" t="s">
-        <v>110</v>
-      </c>
-      <c r="G20" t="s">
-        <v>111</v>
       </c>
       <c r="H20" t="s">
         <v>94</v>
@@ -2636,16 +2636,16 @@
         <v>96</v>
       </c>
       <c r="L20" t="s">
+        <v>111</v>
+      </c>
+      <c r="M20" t="s">
         <v>112</v>
-      </c>
-      <c r="M20" t="s">
-        <v>113</v>
       </c>
       <c r="N20" t="s">
         <v>104</v>
       </c>
       <c r="O20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P20" t="s">
         <v>99</v>
@@ -2657,31 +2657,31 @@
         <v>104</v>
       </c>
       <c r="S20" t="s">
+        <v>113</v>
+      </c>
+      <c r="T20" t="s">
+        <v>99</v>
+      </c>
+      <c r="U20" t="s">
+        <v>99</v>
+      </c>
+      <c r="V20" t="s">
+        <v>100</v>
+      </c>
+      <c r="W20" t="s">
+        <v>100</v>
+      </c>
+      <c r="X20" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA20" t="s">
         <v>114</v>
-      </c>
-      <c r="T20" t="s">
-        <v>99</v>
-      </c>
-      <c r="U20" t="s">
-        <v>99</v>
-      </c>
-      <c r="V20" t="s">
-        <v>100</v>
-      </c>
-      <c r="W20" t="s">
-        <v>100</v>
-      </c>
-      <c r="X20" t="s">
-        <v>99</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>99</v>
-      </c>
-      <c r="Z20" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA20" t="s">
-        <v>115</v>
       </c>
       <c r="AB20" t="s">
         <v>101</v>
@@ -2698,15 +2698,15 @@
     </row>
     <row r="22" spans="1:35">
       <c r="A22" t="s">
+        <v>115</v>
+      </c>
+      <c r="B22" t="s">
         <v>116</v>
-      </c>
-      <c r="B22" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:35">
       <c r="A23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B23" t="s">
         <v>36</v>
@@ -2715,13 +2715,13 @@
         <v>89</v>
       </c>
       <c r="D23" t="s">
+        <v>118</v>
+      </c>
+      <c r="E23" t="s">
         <v>119</v>
       </c>
-      <c r="E23" t="s">
-        <v>120</v>
-      </c>
       <c r="F23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G23" t="s">
         <v>93</v>
@@ -2730,22 +2730,22 @@
         <v>94</v>
       </c>
       <c r="I23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J23" t="s">
         <v>96</v>
       </c>
       <c r="K23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L23" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="M23" t="s">
         <v>100</v>
       </c>
       <c r="N23" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="O23" t="s">
         <v>100</v>
@@ -2757,7 +2757,7 @@
         <v>99</v>
       </c>
       <c r="R23" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="S23" t="s">
         <v>100</v>
@@ -2807,7 +2807,7 @@
     </row>
     <row r="24" spans="1:35">
       <c r="A24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B24" t="s">
         <v>43</v>
@@ -2816,13 +2816,13 @@
         <v>89</v>
       </c>
       <c r="D24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E24" t="s">
         <v>126</v>
       </c>
       <c r="F24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G24" t="s">
         <v>127</v>
@@ -2831,22 +2831,22 @@
         <v>128</v>
       </c>
       <c r="I24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J24" t="s">
         <v>96</v>
       </c>
       <c r="K24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L24" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="M24" t="s">
         <v>100</v>
       </c>
       <c r="N24" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="O24" t="s">
         <v>100</v>
@@ -2858,7 +2858,7 @@
         <v>99</v>
       </c>
       <c r="R24" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="S24" t="s">
         <v>100</v>
@@ -3003,10 +3003,10 @@
         <v>104</v>
       </c>
       <c r="AG27" t="s">
-        <v>136</v>
+        <v>41</v>
       </c>
       <c r="AI27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:35">
@@ -3106,21 +3106,21 @@
     </row>
     <row r="30" spans="1:35">
       <c r="A30" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" t="s">
         <v>137</v>
-      </c>
-      <c r="B30" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:35">
       <c r="A31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B31" t="s">
         <v>36</v>
       </c>
       <c r="C31" t="s">
-        <v>89</v>
+        <v>139</v>
       </c>
       <c r="D31" t="s">
         <v>90</v>
@@ -3210,12 +3210,12 @@
         <v>142</v>
       </c>
       <c r="AI31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:35">
       <c r="A32" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B32" t="s">
         <v>43</v>
@@ -3414,7 +3414,7 @@
         <v>149</v>
       </c>
       <c r="AI35" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:35">
@@ -3440,7 +3440,7 @@
         <v>152</v>
       </c>
       <c r="H36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I36" t="s">
         <v>95</v>
@@ -3497,7 +3497,7 @@
         <v>100</v>
       </c>
       <c r="AA36" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AB36" t="s">
         <v>101</v>
@@ -3531,7 +3531,7 @@
         <v>89</v>
       </c>
       <c r="D39" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E39" t="s">
         <v>156</v>
@@ -3546,13 +3546,13 @@
         <v>94</v>
       </c>
       <c r="I39" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J39" t="s">
         <v>96</v>
       </c>
       <c r="K39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L39" t="s">
         <v>97</v>
@@ -3632,7 +3632,7 @@
         <v>89</v>
       </c>
       <c r="D40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E40" t="s">
         <v>44</v>
@@ -3647,13 +3647,13 @@
         <v>94</v>
       </c>
       <c r="I40" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J40" t="s">
         <v>96</v>
       </c>
       <c r="K40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L40" t="s">
         <v>99</v>
@@ -3756,7 +3756,7 @@
         <v>39</v>
       </c>
       <c r="K43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L43" t="s">
         <v>134</v>
@@ -3819,7 +3819,7 @@
         <v>171</v>
       </c>
       <c r="AG43" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="AI43" t="s">
         <v>172</v>
@@ -3857,7 +3857,7 @@
         <v>39</v>
       </c>
       <c r="K44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L44" t="s">
         <v>134</v>
@@ -4023,7 +4023,7 @@
         <v>184</v>
       </c>
       <c r="AG47" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="AI47" t="s">
         <v>185</v>

</xml_diff>